<commit_message>
first commit in a while for the migration
</commit_message>
<xml_diff>
--- a/data-migration/es_Order_salesforce_fields.xlsx
+++ b/data-migration/es_Order_salesforce_fields.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H580"/>
+  <dimension ref="A1:H581"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16803,27 +16803,27 @@
       </c>
       <c r="B482" t="inlineStr">
         <is>
-          <t>BOM_inside_building_material_total__c</t>
+          <t>Site_Name_No_Spaces__c</t>
         </is>
       </c>
       <c r="C482" t="inlineStr">
         <is>
-          <t>currency</t>
+          <t>string</t>
         </is>
       </c>
       <c r="D482" t="inlineStr">
         <is>
-          <t>BOM Inside Building Material Total</t>
+          <t>Site Name No Spaces</t>
         </is>
       </c>
       <c r="E482" t="n">
-        <v>0</v>
+        <v>1300</v>
       </c>
       <c r="F482" t="b">
         <v>1</v>
       </c>
       <c r="G482" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H482" t="b">
         <v>1</v>
@@ -16837,7 +16837,7 @@
       </c>
       <c r="B483" t="inlineStr">
         <is>
-          <t>BOM_labor_inside_wiring_total__c</t>
+          <t>BOM_inside_building_material_total__c</t>
         </is>
       </c>
       <c r="C483" t="inlineStr">
@@ -16847,7 +16847,7 @@
       </c>
       <c r="D483" t="inlineStr">
         <is>
-          <t>BOM Labor Inside Wiring Total</t>
+          <t>BOM Inside Building Material Total</t>
         </is>
       </c>
       <c r="E483" t="n">
@@ -16871,7 +16871,7 @@
       </c>
       <c r="B484" t="inlineStr">
         <is>
-          <t>BOM_labor_overhead_aerial_total__c</t>
+          <t>BOM_labor_inside_wiring_total__c</t>
         </is>
       </c>
       <c r="C484" t="inlineStr">
@@ -16881,7 +16881,7 @@
       </c>
       <c r="D484" t="inlineStr">
         <is>
-          <t>BOM Labor Overhead Aerial Total</t>
+          <t>BOM Labor Inside Wiring Total</t>
         </is>
       </c>
       <c r="E484" t="n">
@@ -16905,7 +16905,7 @@
       </c>
       <c r="B485" t="inlineStr">
         <is>
-          <t>BOM_labor_underground_total__c</t>
+          <t>BOM_labor_overhead_aerial_total__c</t>
         </is>
       </c>
       <c r="C485" t="inlineStr">
@@ -16915,7 +16915,7 @@
       </c>
       <c r="D485" t="inlineStr">
         <is>
-          <t>BOM Labor Underground Total</t>
+          <t>BOM Labor Overhead Aerial Total</t>
         </is>
       </c>
       <c r="E485" t="n">
@@ -16939,7 +16939,7 @@
       </c>
       <c r="B486" t="inlineStr">
         <is>
-          <t>BOM_misc_total__c</t>
+          <t>BOM_labor_underground_total__c</t>
         </is>
       </c>
       <c r="C486" t="inlineStr">
@@ -16949,7 +16949,7 @@
       </c>
       <c r="D486" t="inlineStr">
         <is>
-          <t>BOM Misc Total</t>
+          <t>BOM Labor Underground Total</t>
         </is>
       </c>
       <c r="E486" t="n">
@@ -16973,7 +16973,7 @@
       </c>
       <c r="B487" t="inlineStr">
         <is>
-          <t>BOM_network_equipment_toal__c</t>
+          <t>BOM_misc_total__c</t>
         </is>
       </c>
       <c r="C487" t="inlineStr">
@@ -16983,7 +16983,7 @@
       </c>
       <c r="D487" t="inlineStr">
         <is>
-          <t>BOM Network Equipment Total</t>
+          <t>BOM Misc Total</t>
         </is>
       </c>
       <c r="E487" t="n">
@@ -17007,7 +17007,7 @@
       </c>
       <c r="B488" t="inlineStr">
         <is>
-          <t>BOM_permitting_total__c</t>
+          <t>BOM_network_equipment_toal__c</t>
         </is>
       </c>
       <c r="C488" t="inlineStr">
@@ -17017,7 +17017,7 @@
       </c>
       <c r="D488" t="inlineStr">
         <is>
-          <t>BOM Permitting Total</t>
+          <t>BOM Network Equipment Total</t>
         </is>
       </c>
       <c r="E488" t="n">
@@ -17041,7 +17041,7 @@
       </c>
       <c r="B489" t="inlineStr">
         <is>
-          <t>BOM_utilities_make_ready_total__c</t>
+          <t>BOM_permitting_total__c</t>
         </is>
       </c>
       <c r="C489" t="inlineStr">
@@ -17051,7 +17051,7 @@
       </c>
       <c r="D489" t="inlineStr">
         <is>
-          <t>BOM Utilities Make Ready Total</t>
+          <t>BOM Permitting Total</t>
         </is>
       </c>
       <c r="E489" t="n">
@@ -17075,24 +17075,24 @@
       </c>
       <c r="B490" t="inlineStr">
         <is>
-          <t>Base_Map_Imported__c</t>
+          <t>BOM_utilities_make_ready_total__c</t>
         </is>
       </c>
       <c r="C490" t="inlineStr">
         <is>
-          <t>boolean</t>
+          <t>currency</t>
         </is>
       </c>
       <c r="D490" t="inlineStr">
         <is>
-          <t>Base Map Imported</t>
+          <t>BOM Utilities Make Ready Total</t>
         </is>
       </c>
       <c r="E490" t="n">
         <v>0</v>
       </c>
       <c r="F490" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G490" t="b">
         <v>0</v>
@@ -17109,7 +17109,7 @@
       </c>
       <c r="B491" t="inlineStr">
         <is>
-          <t>Base_Map_received__c</t>
+          <t>Base_Map_Imported__c</t>
         </is>
       </c>
       <c r="C491" t="inlineStr">
@@ -17119,7 +17119,7 @@
       </c>
       <c r="D491" t="inlineStr">
         <is>
-          <t>Base Map received</t>
+          <t>Base Map Imported</t>
         </is>
       </c>
       <c r="E491" t="n">
@@ -17143,24 +17143,24 @@
       </c>
       <c r="B492" t="inlineStr">
         <is>
-          <t>Core_Provisioning_Complete_Date__c</t>
+          <t>Base_Map_received__c</t>
         </is>
       </c>
       <c r="C492" t="inlineStr">
         <is>
-          <t>date</t>
+          <t>boolean</t>
         </is>
       </c>
       <c r="D492" t="inlineStr">
         <is>
-          <t>Core Provisioning Complete Date</t>
+          <t>Base Map received</t>
         </is>
       </c>
       <c r="E492" t="n">
         <v>0</v>
       </c>
       <c r="F492" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G492" t="b">
         <v>0</v>
@@ -17177,7 +17177,7 @@
       </c>
       <c r="B493" t="inlineStr">
         <is>
-          <t>Construction_Completion_Date__c</t>
+          <t>Core_Provisioning_Complete_Date__c</t>
         </is>
       </c>
       <c r="C493" t="inlineStr">
@@ -17187,7 +17187,7 @@
       </c>
       <c r="D493" t="inlineStr">
         <is>
-          <t>Construction Completion Date (CCD)</t>
+          <t>Core Provisioning Complete Date</t>
         </is>
       </c>
       <c r="E493" t="n">
@@ -17211,17 +17211,17 @@
       </c>
       <c r="B494" t="inlineStr">
         <is>
-          <t>Construction_Materials_Total__c</t>
+          <t>Construction_Completion_Date__c</t>
         </is>
       </c>
       <c r="C494" t="inlineStr">
         <is>
-          <t>currency</t>
+          <t>date</t>
         </is>
       </c>
       <c r="D494" t="inlineStr">
         <is>
-          <t>Construction Material Total (Deprecated)</t>
+          <t>Construction Completion Date (CCD)</t>
         </is>
       </c>
       <c r="E494" t="n">
@@ -17245,21 +17245,21 @@
       </c>
       <c r="B495" t="inlineStr">
         <is>
-          <t>Construction_Status__c</t>
+          <t>Construction_Materials_Total__c</t>
         </is>
       </c>
       <c r="C495" t="inlineStr">
         <is>
-          <t>picklist</t>
+          <t>currency</t>
         </is>
       </c>
       <c r="D495" t="inlineStr">
         <is>
-          <t>Construction Status</t>
+          <t>Construction Material Total (Deprecated)</t>
         </is>
       </c>
       <c r="E495" t="n">
-        <v>255</v>
+        <v>0</v>
       </c>
       <c r="F495" t="b">
         <v>1</v>
@@ -17279,21 +17279,21 @@
       </c>
       <c r="B496" t="inlineStr">
         <is>
-          <t>Contractor__c</t>
+          <t>Construction_Status__c</t>
         </is>
       </c>
       <c r="C496" t="inlineStr">
         <is>
-          <t>reference</t>
+          <t>picklist</t>
         </is>
       </c>
       <c r="D496" t="inlineStr">
         <is>
-          <t>Contractor</t>
+          <t>Construction Status</t>
         </is>
       </c>
       <c r="E496" t="n">
-        <v>18</v>
+        <v>255</v>
       </c>
       <c r="F496" t="b">
         <v>1</v>
@@ -17313,27 +17313,27 @@
       </c>
       <c r="B497" t="inlineStr">
         <is>
-          <t>Customer_Touch_Jeopardy_Projects__c</t>
+          <t>Contractor__c</t>
         </is>
       </c>
       <c r="C497" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>reference</t>
         </is>
       </c>
       <c r="D497" t="inlineStr">
         <is>
-          <t>Customer Touch Jeopardy Projects</t>
+          <t>Contractor</t>
         </is>
       </c>
       <c r="E497" t="n">
-        <v>1300</v>
+        <v>18</v>
       </c>
       <c r="F497" t="b">
         <v>1</v>
       </c>
       <c r="G497" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H497" t="b">
         <v>1</v>
@@ -17347,7 +17347,7 @@
       </c>
       <c r="B498" t="inlineStr">
         <is>
-          <t>Customer_Touch_Point_On_Track_Projects__c</t>
+          <t>Customer_Touch_Jeopardy_Projects__c</t>
         </is>
       </c>
       <c r="C498" t="inlineStr">
@@ -17357,7 +17357,7 @@
       </c>
       <c r="D498" t="inlineStr">
         <is>
-          <t>Customer Touch Point On Track Projects</t>
+          <t>Customer Touch Jeopardy Projects</t>
         </is>
       </c>
       <c r="E498" t="n">
@@ -17381,21 +17381,21 @@
       </c>
       <c r="B499" t="inlineStr">
         <is>
-          <t>Days_between_CCD_and_ECD__c</t>
+          <t>Customer_Touch_Point_On_Track_Projects__c</t>
         </is>
       </c>
       <c r="C499" t="inlineStr">
         <is>
-          <t>double</t>
+          <t>string</t>
         </is>
       </c>
       <c r="D499" t="inlineStr">
         <is>
-          <t>Days between CCD and ECD</t>
+          <t>Customer Touch Point On Track Projects</t>
         </is>
       </c>
       <c r="E499" t="n">
-        <v>0</v>
+        <v>1300</v>
       </c>
       <c r="F499" t="b">
         <v>1</v>
@@ -17415,7 +17415,7 @@
       </c>
       <c r="B500" t="inlineStr">
         <is>
-          <t>Days_to_Order_Confirmation__c</t>
+          <t>Days_between_CCD_and_ECD__c</t>
         </is>
       </c>
       <c r="C500" t="inlineStr">
@@ -17425,7 +17425,7 @@
       </c>
       <c r="D500" t="inlineStr">
         <is>
-          <t>Days to Order Confirmation</t>
+          <t>Days between CCD and ECD</t>
         </is>
       </c>
       <c r="E500" t="n">
@@ -17449,27 +17449,27 @@
       </c>
       <c r="B501" t="inlineStr">
         <is>
-          <t>Design_Package_Status__c</t>
+          <t>Days_to_Order_Confirmation__c</t>
         </is>
       </c>
       <c r="C501" t="inlineStr">
         <is>
-          <t>picklist</t>
+          <t>double</t>
         </is>
       </c>
       <c r="D501" t="inlineStr">
         <is>
-          <t>Design Package Status (Deprecated)</t>
+          <t>Days to Order Confirmation</t>
         </is>
       </c>
       <c r="E501" t="n">
-        <v>255</v>
+        <v>0</v>
       </c>
       <c r="F501" t="b">
         <v>1</v>
       </c>
       <c r="G501" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H501" t="b">
         <v>1</v>
@@ -17483,21 +17483,21 @@
       </c>
       <c r="B502" t="inlineStr">
         <is>
-          <t>Design_Request_Received__c</t>
+          <t>Design_Package_Status__c</t>
         </is>
       </c>
       <c r="C502" t="inlineStr">
         <is>
-          <t>date</t>
+          <t>picklist</t>
         </is>
       </c>
       <c r="D502" t="inlineStr">
         <is>
-          <t>Design Request Received (Deprecated)</t>
+          <t>Design Package Status (Deprecated)</t>
         </is>
       </c>
       <c r="E502" t="n">
-        <v>0</v>
+        <v>255</v>
       </c>
       <c r="F502" t="b">
         <v>1</v>
@@ -17517,7 +17517,7 @@
       </c>
       <c r="B503" t="inlineStr">
         <is>
-          <t>Designs_Completed_Date__c</t>
+          <t>Design_Request_Received__c</t>
         </is>
       </c>
       <c r="C503" t="inlineStr">
@@ -17527,7 +17527,7 @@
       </c>
       <c r="D503" t="inlineStr">
         <is>
-          <t>Designs Completed Date</t>
+          <t>Design Request Received (Deprecated)</t>
         </is>
       </c>
       <c r="E503" t="n">
@@ -17551,21 +17551,21 @@
       </c>
       <c r="B504" t="inlineStr">
         <is>
-          <t>Facility__c</t>
+          <t>Designs_Completed_Date__c</t>
         </is>
       </c>
       <c r="C504" t="inlineStr">
         <is>
-          <t>reference</t>
+          <t>date</t>
         </is>
       </c>
       <c r="D504" t="inlineStr">
         <is>
-          <t>Facility - Address A</t>
+          <t>Designs Completed Date</t>
         </is>
       </c>
       <c r="E504" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="F504" t="b">
         <v>1</v>
@@ -17585,24 +17585,24 @@
       </c>
       <c r="B505" t="inlineStr">
         <is>
-          <t>Fast_Track__c</t>
+          <t>Facility__c</t>
         </is>
       </c>
       <c r="C505" t="inlineStr">
         <is>
-          <t>boolean</t>
+          <t>reference</t>
         </is>
       </c>
       <c r="D505" t="inlineStr">
         <is>
-          <t>Fast Track</t>
+          <t>Facility - Address A</t>
         </is>
       </c>
       <c r="E505" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="F505" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G505" t="b">
         <v>0</v>
@@ -17619,24 +17619,24 @@
       </c>
       <c r="B506" t="inlineStr">
         <is>
-          <t>Fiber_Optic_Cable_Total__c</t>
+          <t>Fast_Track__c</t>
         </is>
       </c>
       <c r="C506" t="inlineStr">
         <is>
-          <t>currency</t>
+          <t>boolean</t>
         </is>
       </c>
       <c r="D506" t="inlineStr">
         <is>
-          <t>Fiber Optic Cable Total (Deprecated)</t>
+          <t>Fast Track</t>
         </is>
       </c>
       <c r="E506" t="n">
         <v>0</v>
       </c>
       <c r="F506" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G506" t="b">
         <v>0</v>
@@ -17653,21 +17653,21 @@
       </c>
       <c r="B507" t="inlineStr">
         <is>
-          <t>IRU_Access__c</t>
+          <t>Fiber_Optic_Cable_Total__c</t>
         </is>
       </c>
       <c r="C507" t="inlineStr">
         <is>
-          <t>picklist</t>
+          <t>currency</t>
         </is>
       </c>
       <c r="D507" t="inlineStr">
         <is>
-          <t>IRU Access</t>
+          <t>Fiber Optic Cable Total (Deprecated)</t>
         </is>
       </c>
       <c r="E507" t="n">
-        <v>255</v>
+        <v>0</v>
       </c>
       <c r="F507" t="b">
         <v>1</v>
@@ -17687,21 +17687,21 @@
       </c>
       <c r="B508" t="inlineStr">
         <is>
-          <t>Fiber_Design_Complete_Date__c</t>
+          <t>IRU_Access__c</t>
         </is>
       </c>
       <c r="C508" t="inlineStr">
         <is>
-          <t>date</t>
+          <t>picklist</t>
         </is>
       </c>
       <c r="D508" t="inlineStr">
         <is>
-          <t>Fiber Design Complete Date</t>
+          <t>IRU Access</t>
         </is>
       </c>
       <c r="E508" t="n">
-        <v>0</v>
+        <v>255</v>
       </c>
       <c r="F508" t="b">
         <v>1</v>
@@ -17721,7 +17721,7 @@
       </c>
       <c r="B509" t="inlineStr">
         <is>
-          <t>LL_Ntp_Received__c</t>
+          <t>Fiber_Design_Complete_Date__c</t>
         </is>
       </c>
       <c r="C509" t="inlineStr">
@@ -17731,7 +17731,7 @@
       </c>
       <c r="D509" t="inlineStr">
         <is>
-          <t>LL NTP Received</t>
+          <t>Fiber Design Complete Date</t>
         </is>
       </c>
       <c r="E509" t="n">
@@ -17755,7 +17755,7 @@
       </c>
       <c r="B510" t="inlineStr">
         <is>
-          <t>Design_Imported_GIS_Date__c</t>
+          <t>LL_Ntp_Received__c</t>
         </is>
       </c>
       <c r="C510" t="inlineStr">
@@ -17765,7 +17765,7 @@
       </c>
       <c r="D510" t="inlineStr">
         <is>
-          <t>Design Imported (GIS) Date</t>
+          <t>LL NTP Received</t>
         </is>
       </c>
       <c r="E510" t="n">
@@ -17789,7 +17789,7 @@
       </c>
       <c r="B511" t="inlineStr">
         <is>
-          <t>Construction_Complete_Status_Date__c</t>
+          <t>Design_Imported_GIS_Date__c</t>
         </is>
       </c>
       <c r="C511" t="inlineStr">
@@ -17799,7 +17799,7 @@
       </c>
       <c r="D511" t="inlineStr">
         <is>
-          <t>Construction Complete Status Date</t>
+          <t>Design Imported (GIS) Date</t>
         </is>
       </c>
       <c r="E511" t="n">
@@ -17823,27 +17823,27 @@
       </c>
       <c r="B512" t="inlineStr">
         <is>
-          <t>OSP_Task_logical__c</t>
+          <t>Construction_Complete_Status_Date__c</t>
         </is>
       </c>
       <c r="C512" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>date</t>
         </is>
       </c>
       <c r="D512" t="inlineStr">
         <is>
-          <t>OSP Task logical</t>
+          <t>Construction Complete Status Date</t>
         </is>
       </c>
       <c r="E512" t="n">
-        <v>1300</v>
+        <v>0</v>
       </c>
       <c r="F512" t="b">
         <v>1</v>
       </c>
       <c r="G512" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H512" t="b">
         <v>1</v>
@@ -17857,21 +17857,21 @@
       </c>
       <c r="B513" t="inlineStr">
         <is>
-          <t>ECD_then_BSD_Reporting__c</t>
+          <t>OSP_Task_logical__c</t>
         </is>
       </c>
       <c r="C513" t="inlineStr">
         <is>
-          <t>date</t>
+          <t>string</t>
         </is>
       </c>
       <c r="D513" t="inlineStr">
         <is>
-          <t>ECD then BSD (Reporting)</t>
+          <t>OSP Task logical</t>
         </is>
       </c>
       <c r="E513" t="n">
-        <v>0</v>
+        <v>1300</v>
       </c>
       <c r="F513" t="b">
         <v>1</v>
@@ -17891,24 +17891,24 @@
       </c>
       <c r="B514" t="inlineStr">
         <is>
-          <t>All_Permits_Completed__c</t>
+          <t>ECD_then_BSD_Reporting__c</t>
         </is>
       </c>
       <c r="C514" t="inlineStr">
         <is>
-          <t>boolean</t>
+          <t>date</t>
         </is>
       </c>
       <c r="D514" t="inlineStr">
         <is>
-          <t>All Permits Completed</t>
+          <t>ECD then BSD (Reporting)</t>
         </is>
       </c>
       <c r="E514" t="n">
         <v>0</v>
       </c>
       <c r="F514" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G514" t="b">
         <v>1</v>
@@ -17925,27 +17925,27 @@
       </c>
       <c r="B515" t="inlineStr">
         <is>
-          <t>NTP_Request_Submitted__c</t>
+          <t>All_Permits_Completed__c</t>
         </is>
       </c>
       <c r="C515" t="inlineStr">
         <is>
-          <t>date</t>
+          <t>boolean</t>
         </is>
       </c>
       <c r="D515" t="inlineStr">
         <is>
-          <t>Deprecated</t>
+          <t>All Permits Completed</t>
         </is>
       </c>
       <c r="E515" t="n">
         <v>0</v>
       </c>
       <c r="F515" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G515" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H515" t="b">
         <v>1</v>
@@ -17959,21 +17959,21 @@
       </c>
       <c r="B516" t="inlineStr">
         <is>
-          <t>Design_Layout_For_Formula__c</t>
+          <t>NTP_Request_Submitted__c</t>
         </is>
       </c>
       <c r="C516" t="inlineStr">
         <is>
-          <t>reference</t>
+          <t>date</t>
         </is>
       </c>
       <c r="D516" t="inlineStr">
         <is>
-          <t>Design Layout For Formula</t>
+          <t>Deprecated</t>
         </is>
       </c>
       <c r="E516" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="F516" t="b">
         <v>1</v>
@@ -17993,21 +17993,21 @@
       </c>
       <c r="B517" t="inlineStr">
         <is>
-          <t>OSPE_Walkout_Date__c</t>
+          <t>Design_Layout_For_Formula__c</t>
         </is>
       </c>
       <c r="C517" t="inlineStr">
         <is>
-          <t>date</t>
+          <t>reference</t>
         </is>
       </c>
       <c r="D517" t="inlineStr">
         <is>
-          <t>OSPE Walkout Date</t>
+          <t>Design Layout For Formula</t>
         </is>
       </c>
       <c r="E517" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="F517" t="b">
         <v>1</v>
@@ -18027,24 +18027,24 @@
       </c>
       <c r="B518" t="inlineStr">
         <is>
-          <t>OSP_DEsign_Imported__c</t>
+          <t>OSPE_Walkout_Date__c</t>
         </is>
       </c>
       <c r="C518" t="inlineStr">
         <is>
-          <t>boolean</t>
+          <t>date</t>
         </is>
       </c>
       <c r="D518" t="inlineStr">
         <is>
-          <t>Design Drafted in 3GIS</t>
+          <t>OSPE Walkout Date</t>
         </is>
       </c>
       <c r="E518" t="n">
         <v>0</v>
       </c>
       <c r="F518" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G518" t="b">
         <v>0</v>
@@ -18061,7 +18061,7 @@
       </c>
       <c r="B519" t="inlineStr">
         <is>
-          <t>OSP_DEsign_Received__c</t>
+          <t>OSP_DEsign_Imported__c</t>
         </is>
       </c>
       <c r="C519" t="inlineStr">
@@ -18071,7 +18071,7 @@
       </c>
       <c r="D519" t="inlineStr">
         <is>
-          <t>Design Provided for 3GIS (OSP)</t>
+          <t>Design Drafted in 3GIS</t>
         </is>
       </c>
       <c r="E519" t="n">
@@ -18095,7 +18095,7 @@
       </c>
       <c r="B520" t="inlineStr">
         <is>
-          <t>OSP_Design_Revised__c</t>
+          <t>OSP_DEsign_Received__c</t>
         </is>
       </c>
       <c r="C520" t="inlineStr">
@@ -18105,7 +18105,7 @@
       </c>
       <c r="D520" t="inlineStr">
         <is>
-          <t>Revised Design for 3GIS</t>
+          <t>Design Provided for 3GIS (OSP)</t>
         </is>
       </c>
       <c r="E520" t="n">
@@ -18129,24 +18129,24 @@
       </c>
       <c r="B521" t="inlineStr">
         <is>
-          <t>OSP_Notes__c</t>
+          <t>OSP_Design_Revised__c</t>
         </is>
       </c>
       <c r="C521" t="inlineStr">
         <is>
-          <t>textarea</t>
+          <t>boolean</t>
         </is>
       </c>
       <c r="D521" t="inlineStr">
         <is>
-          <t>OSP Notes</t>
+          <t>Revised Design for 3GIS</t>
         </is>
       </c>
       <c r="E521" t="n">
-        <v>32768</v>
+        <v>0</v>
       </c>
       <c r="F521" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G521" t="b">
         <v>0</v>
@@ -18163,24 +18163,24 @@
       </c>
       <c r="B522" t="inlineStr">
         <is>
-          <t>OTDR_Complete__c</t>
+          <t>OSP_Notes__c</t>
         </is>
       </c>
       <c r="C522" t="inlineStr">
         <is>
-          <t>boolean</t>
+          <t>textarea</t>
         </is>
       </c>
       <c r="D522" t="inlineStr">
         <is>
-          <t>OTDR Complete</t>
+          <t>OSP Notes</t>
         </is>
       </c>
       <c r="E522" t="n">
-        <v>0</v>
+        <v>32768</v>
       </c>
       <c r="F522" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G522" t="b">
         <v>0</v>
@@ -18197,24 +18197,24 @@
       </c>
       <c r="B523" t="inlineStr">
         <is>
-          <t>OTDR_Distance__c</t>
+          <t>OTDR_Complete__c</t>
         </is>
       </c>
       <c r="C523" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>boolean</t>
         </is>
       </c>
       <c r="D523" t="inlineStr">
         <is>
-          <t>OTDR Distance</t>
+          <t>OTDR Complete</t>
         </is>
       </c>
       <c r="E523" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F523" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G523" t="b">
         <v>0</v>
@@ -18231,7 +18231,7 @@
       </c>
       <c r="B524" t="inlineStr">
         <is>
-          <t>OTDR_Loss__c</t>
+          <t>OTDR_Distance__c</t>
         </is>
       </c>
       <c r="C524" t="inlineStr">
@@ -18241,7 +18241,7 @@
       </c>
       <c r="D524" t="inlineStr">
         <is>
-          <t>OTDR Loss</t>
+          <t>OTDR Distance</t>
         </is>
       </c>
       <c r="E524" t="n">
@@ -18265,21 +18265,21 @@
       </c>
       <c r="B525" t="inlineStr">
         <is>
-          <t>Order_Confirmation_Sent_Date__c</t>
+          <t>OTDR_Loss__c</t>
         </is>
       </c>
       <c r="C525" t="inlineStr">
         <is>
-          <t>date</t>
+          <t>string</t>
         </is>
       </c>
       <c r="D525" t="inlineStr">
         <is>
-          <t>Order Confirmation Sent Date</t>
+          <t>OTDR Loss</t>
         </is>
       </c>
       <c r="E525" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="F525" t="b">
         <v>1</v>
@@ -18299,21 +18299,21 @@
       </c>
       <c r="B526" t="inlineStr">
         <is>
-          <t>Order_Phase__c</t>
+          <t>Order_Confirmation_Sent_Date__c</t>
         </is>
       </c>
       <c r="C526" t="inlineStr">
         <is>
-          <t>picklist</t>
+          <t>date</t>
         </is>
       </c>
       <c r="D526" t="inlineStr">
         <is>
-          <t>Order Phase</t>
+          <t>Order Confirmation Sent Date</t>
         </is>
       </c>
       <c r="E526" t="n">
-        <v>255</v>
+        <v>0</v>
       </c>
       <c r="F526" t="b">
         <v>1</v>
@@ -18333,27 +18333,27 @@
       </c>
       <c r="B527" t="inlineStr">
         <is>
-          <t>Permit_Approved__c</t>
+          <t>Order_Phase__c</t>
         </is>
       </c>
       <c r="C527" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>picklist</t>
         </is>
       </c>
       <c r="D527" t="inlineStr">
         <is>
-          <t>Permit Approved Flag</t>
+          <t>Order Phase</t>
         </is>
       </c>
       <c r="E527" t="n">
-        <v>1300</v>
+        <v>255</v>
       </c>
       <c r="F527" t="b">
         <v>1</v>
       </c>
       <c r="G527" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H527" t="b">
         <v>1</v>
@@ -18367,27 +18367,27 @@
       </c>
       <c r="B528" t="inlineStr">
         <is>
-          <t>ECD_Change_Counter__c</t>
+          <t>Permit_Approved__c</t>
         </is>
       </c>
       <c r="C528" t="inlineStr">
         <is>
-          <t>double</t>
+          <t>string</t>
         </is>
       </c>
       <c r="D528" t="inlineStr">
         <is>
-          <t>ECD Change Counter</t>
+          <t>Permit Approved Flag</t>
         </is>
       </c>
       <c r="E528" t="n">
-        <v>0</v>
+        <v>1300</v>
       </c>
       <c r="F528" t="b">
         <v>1</v>
       </c>
       <c r="G528" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H528" t="b">
         <v>1</v>
@@ -18401,17 +18401,17 @@
       </c>
       <c r="B529" t="inlineStr">
         <is>
-          <t>Phase_Milestone_Fiber_Coiled_at_Curb__c</t>
+          <t>ECD_Change_Counter__c</t>
         </is>
       </c>
       <c r="C529" t="inlineStr">
         <is>
-          <t>date</t>
+          <t>double</t>
         </is>
       </c>
       <c r="D529" t="inlineStr">
         <is>
-          <t>Phase Milestone Fiber Coiled at Curb</t>
+          <t>ECD Change Counter</t>
         </is>
       </c>
       <c r="E529" t="n">
@@ -18435,21 +18435,21 @@
       </c>
       <c r="B530" t="inlineStr">
         <is>
-          <t>IRU_Owner__c</t>
+          <t>Phase_Milestone_Fiber_Coiled_at_Curb__c</t>
         </is>
       </c>
       <c r="C530" t="inlineStr">
         <is>
-          <t>picklist</t>
+          <t>date</t>
         </is>
       </c>
       <c r="D530" t="inlineStr">
         <is>
-          <t>IRU Owner</t>
+          <t>Phase Milestone Fiber Coiled at Curb</t>
         </is>
       </c>
       <c r="E530" t="n">
-        <v>255</v>
+        <v>0</v>
       </c>
       <c r="F530" t="b">
         <v>1</v>
@@ -18469,21 +18469,21 @@
       </c>
       <c r="B531" t="inlineStr">
         <is>
-          <t>Project_Module__c</t>
+          <t>IRU_Owner__c</t>
         </is>
       </c>
       <c r="C531" t="inlineStr">
         <is>
-          <t>reference</t>
+          <t>picklist</t>
         </is>
       </c>
       <c r="D531" t="inlineStr">
         <is>
-          <t>Project Module</t>
+          <t>IRU Owner</t>
         </is>
       </c>
       <c r="E531" t="n">
-        <v>18</v>
+        <v>255</v>
       </c>
       <c r="F531" t="b">
         <v>1</v>
@@ -18503,21 +18503,21 @@
       </c>
       <c r="B532" t="inlineStr">
         <is>
-          <t>Hold_Reason_Notes__c</t>
+          <t>Project_Module__c</t>
         </is>
       </c>
       <c r="C532" t="inlineStr">
         <is>
-          <t>textarea</t>
+          <t>reference</t>
         </is>
       </c>
       <c r="D532" t="inlineStr">
         <is>
-          <t>Hold Reason Notes</t>
+          <t>Project Module</t>
         </is>
       </c>
       <c r="E532" t="n">
-        <v>131000</v>
+        <v>18</v>
       </c>
       <c r="F532" t="b">
         <v>1</v>
@@ -18537,21 +18537,21 @@
       </c>
       <c r="B533" t="inlineStr">
         <is>
-          <t>Quote_Vendor_Name__c</t>
+          <t>Hold_Reason_Notes__c</t>
         </is>
       </c>
       <c r="C533" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>textarea</t>
         </is>
       </c>
       <c r="D533" t="inlineStr">
         <is>
-          <t>OFF-NET Quote : Vendor Name</t>
+          <t>Hold Reason Notes</t>
         </is>
       </c>
       <c r="E533" t="n">
-        <v>80</v>
+        <v>131000</v>
       </c>
       <c r="F533" t="b">
         <v>1</v>
@@ -18571,7 +18571,7 @@
       </c>
       <c r="B534" t="inlineStr">
         <is>
-          <t>Account_Link__c</t>
+          <t>Quote_Vendor_Name__c</t>
         </is>
       </c>
       <c r="C534" t="inlineStr">
@@ -18581,17 +18581,17 @@
       </c>
       <c r="D534" t="inlineStr">
         <is>
-          <t>Account Link</t>
+          <t>OFF-NET Quote : Vendor Name</t>
         </is>
       </c>
       <c r="E534" t="n">
-        <v>1300</v>
+        <v>80</v>
       </c>
       <c r="F534" t="b">
         <v>1</v>
       </c>
       <c r="G534" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H534" t="b">
         <v>1</v>
@@ -18605,7 +18605,7 @@
       </c>
       <c r="B535" t="inlineStr">
         <is>
-          <t>Site_Name_Address_A__c</t>
+          <t>Account_Link__c</t>
         </is>
       </c>
       <c r="C535" t="inlineStr">
@@ -18615,17 +18615,17 @@
       </c>
       <c r="D535" t="inlineStr">
         <is>
-          <t>Site Name Address A</t>
+          <t>Account Link</t>
         </is>
       </c>
       <c r="E535" t="n">
-        <v>100</v>
+        <v>1300</v>
       </c>
       <c r="F535" t="b">
         <v>1</v>
       </c>
       <c r="G535" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H535" t="b">
         <v>1</v>
@@ -18639,7 +18639,7 @@
       </c>
       <c r="B536" t="inlineStr">
         <is>
-          <t>Selected_Headend_Type__c</t>
+          <t>Site_Name_Address_A__c</t>
         </is>
       </c>
       <c r="C536" t="inlineStr">
@@ -18649,17 +18649,17 @@
       </c>
       <c r="D536" t="inlineStr">
         <is>
-          <t>Selected Headend Type</t>
+          <t>Site Name Address A</t>
         </is>
       </c>
       <c r="E536" t="n">
-        <v>1300</v>
+        <v>100</v>
       </c>
       <c r="F536" t="b">
         <v>1</v>
       </c>
       <c r="G536" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H536" t="b">
         <v>1</v>
@@ -18673,27 +18673,27 @@
       </c>
       <c r="B537" t="inlineStr">
         <is>
-          <t>Site_Contact_Email__c</t>
+          <t>Selected_Headend_Type__c</t>
         </is>
       </c>
       <c r="C537" t="inlineStr">
         <is>
-          <t>email</t>
+          <t>string</t>
         </is>
       </c>
       <c r="D537" t="inlineStr">
         <is>
-          <t>Site Contact: Email</t>
+          <t>Selected Headend Type</t>
         </is>
       </c>
       <c r="E537" t="n">
-        <v>80</v>
+        <v>1300</v>
       </c>
       <c r="F537" t="b">
         <v>1</v>
       </c>
       <c r="G537" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H537" t="b">
         <v>1</v>
@@ -18707,21 +18707,21 @@
       </c>
       <c r="B538" t="inlineStr">
         <is>
-          <t>Site_Contact_Phone__c</t>
+          <t>Site_Contact_Email__c</t>
         </is>
       </c>
       <c r="C538" t="inlineStr">
         <is>
-          <t>phone</t>
+          <t>email</t>
         </is>
       </c>
       <c r="D538" t="inlineStr">
         <is>
-          <t>Site Contact: Phone</t>
+          <t>Site Contact: Email</t>
         </is>
       </c>
       <c r="E538" t="n">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="F538" t="b">
         <v>1</v>
@@ -18741,21 +18741,21 @@
       </c>
       <c r="B539" t="inlineStr">
         <is>
-          <t>Site_Contact_Preferred_Method__c</t>
+          <t>Site_Contact_Phone__c</t>
         </is>
       </c>
       <c r="C539" t="inlineStr">
         <is>
-          <t>picklist</t>
+          <t>phone</t>
         </is>
       </c>
       <c r="D539" t="inlineStr">
         <is>
-          <t>Site Contact: Pref Method</t>
+          <t>Site Contact: Phone</t>
         </is>
       </c>
       <c r="E539" t="n">
-        <v>255</v>
+        <v>40</v>
       </c>
       <c r="F539" t="b">
         <v>1</v>
@@ -18775,17 +18775,17 @@
       </c>
       <c r="B540" t="inlineStr">
         <is>
-          <t>Site_Contact__c</t>
+          <t>Site_Contact_Preferred_Method__c</t>
         </is>
       </c>
       <c r="C540" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>picklist</t>
         </is>
       </c>
       <c r="D540" t="inlineStr">
         <is>
-          <t>Site Contact</t>
+          <t>Site Contact: Pref Method</t>
         </is>
       </c>
       <c r="E540" t="n">
@@ -18809,21 +18809,21 @@
       </c>
       <c r="B541" t="inlineStr">
         <is>
-          <t>Site_Contacted__c</t>
+          <t>Site_Contact__c</t>
         </is>
       </c>
       <c r="C541" t="inlineStr">
         <is>
-          <t>date</t>
+          <t>string</t>
         </is>
       </c>
       <c r="D541" t="inlineStr">
         <is>
-          <t>Site Contacted</t>
+          <t>Site Contact</t>
         </is>
       </c>
       <c r="E541" t="n">
-        <v>0</v>
+        <v>255</v>
       </c>
       <c r="F541" t="b">
         <v>1</v>
@@ -18843,7 +18843,7 @@
       </c>
       <c r="B542" t="inlineStr">
         <is>
-          <t>Site_Received__c</t>
+          <t>Site_Contacted__c</t>
         </is>
       </c>
       <c r="C542" t="inlineStr">
@@ -18853,7 +18853,7 @@
       </c>
       <c r="D542" t="inlineStr">
         <is>
-          <t>Site Received</t>
+          <t>Site Contacted</t>
         </is>
       </c>
       <c r="E542" t="n">
@@ -18877,7 +18877,7 @@
       </c>
       <c r="B543" t="inlineStr">
         <is>
-          <t>Site_Survey_Complete__c</t>
+          <t>Site_Received__c</t>
         </is>
       </c>
       <c r="C543" t="inlineStr">
@@ -18887,7 +18887,7 @@
       </c>
       <c r="D543" t="inlineStr">
         <is>
-          <t>Site Survey Complete</t>
+          <t>Site Received</t>
         </is>
       </c>
       <c r="E543" t="n">
@@ -18911,7 +18911,7 @@
       </c>
       <c r="B544" t="inlineStr">
         <is>
-          <t>Site_Survey_Scheduled__c</t>
+          <t>Site_Survey_Complete__c</t>
         </is>
       </c>
       <c r="C544" t="inlineStr">
@@ -18921,7 +18921,7 @@
       </c>
       <c r="D544" t="inlineStr">
         <is>
-          <t>Date of Site Survey</t>
+          <t>Site Survey Complete</t>
         </is>
       </c>
       <c r="E544" t="n">
@@ -18945,21 +18945,21 @@
       </c>
       <c r="B545" t="inlineStr">
         <is>
-          <t>Small_Cell_Contractor__c</t>
+          <t>Site_Survey_Scheduled__c</t>
         </is>
       </c>
       <c r="C545" t="inlineStr">
         <is>
-          <t>reference</t>
+          <t>date</t>
         </is>
       </c>
       <c r="D545" t="inlineStr">
         <is>
-          <t>Small Cell Contractor</t>
+          <t>Date of Site Survey</t>
         </is>
       </c>
       <c r="E545" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="F545" t="b">
         <v>1</v>
@@ -18979,24 +18979,24 @@
       </c>
       <c r="B546" t="inlineStr">
         <is>
-          <t>LOA_CFA_Required__c</t>
+          <t>Small_Cell_Contractor__c</t>
         </is>
       </c>
       <c r="C546" t="inlineStr">
         <is>
-          <t>boolean</t>
+          <t>reference</t>
         </is>
       </c>
       <c r="D546" t="inlineStr">
         <is>
-          <t>Address A: LOA/CFA Required</t>
+          <t>Small Cell Contractor</t>
         </is>
       </c>
       <c r="E546" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="F546" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G546" t="b">
         <v>0</v>
@@ -19013,7 +19013,7 @@
       </c>
       <c r="B547" t="inlineStr">
         <is>
-          <t>Splice_Documents_Received__c</t>
+          <t>LOA_CFA_Required__c</t>
         </is>
       </c>
       <c r="C547" t="inlineStr">
@@ -19023,7 +19023,7 @@
       </c>
       <c r="D547" t="inlineStr">
         <is>
-          <t>As Spliced Docs Received (OSP)</t>
+          <t>Address A: LOA/CFA Required</t>
         </is>
       </c>
       <c r="E547" t="n">
@@ -19047,24 +19047,24 @@
       </c>
       <c r="B548" t="inlineStr">
         <is>
-          <t>Status_ROE__c</t>
+          <t>Splice_Documents_Received__c</t>
         </is>
       </c>
       <c r="C548" t="inlineStr">
         <is>
-          <t>picklist</t>
+          <t>boolean</t>
         </is>
       </c>
       <c r="D548" t="inlineStr">
         <is>
-          <t>Status ROE</t>
+          <t>As Spliced Docs Received (OSP)</t>
         </is>
       </c>
       <c r="E548" t="n">
-        <v>255</v>
+        <v>0</v>
       </c>
       <c r="F548" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G548" t="b">
         <v>0</v>
@@ -19081,21 +19081,21 @@
       </c>
       <c r="B549" t="inlineStr">
         <is>
-          <t>Utilities_Make_Ready_Total__c</t>
+          <t>Status_ROE__c</t>
         </is>
       </c>
       <c r="C549" t="inlineStr">
         <is>
-          <t>currency</t>
+          <t>picklist</t>
         </is>
       </c>
       <c r="D549" t="inlineStr">
         <is>
-          <t>Utilities Make Ready Total (Deprecated)</t>
+          <t>Status ROE</t>
         </is>
       </c>
       <c r="E549" t="n">
-        <v>0</v>
+        <v>255</v>
       </c>
       <c r="F549" t="b">
         <v>1</v>
@@ -19115,17 +19115,17 @@
       </c>
       <c r="B550" t="inlineStr">
         <is>
-          <t>Walkout_Completed__c</t>
+          <t>Utilities_Make_Ready_Total__c</t>
         </is>
       </c>
       <c r="C550" t="inlineStr">
         <is>
-          <t>datetime</t>
+          <t>currency</t>
         </is>
       </c>
       <c r="D550" t="inlineStr">
         <is>
-          <t>Walkout Completed</t>
+          <t>Utilities Make Ready Total (Deprecated)</t>
         </is>
       </c>
       <c r="E550" t="n">
@@ -19149,17 +19149,17 @@
       </c>
       <c r="B551" t="inlineStr">
         <is>
-          <t>Wireless_Customer_NTP__c</t>
+          <t>Walkout_Completed__c</t>
         </is>
       </c>
       <c r="C551" t="inlineStr">
         <is>
-          <t>date</t>
+          <t>datetime</t>
         </is>
       </c>
       <c r="D551" t="inlineStr">
         <is>
-          <t>Wireless Customer NTP</t>
+          <t>Walkout Completed</t>
         </is>
       </c>
       <c r="E551" t="n">
@@ -19183,7 +19183,7 @@
       </c>
       <c r="B552" t="inlineStr">
         <is>
-          <t>Wireless_Customer_Telco_Ready__c</t>
+          <t>Wireless_Customer_NTP__c</t>
         </is>
       </c>
       <c r="C552" t="inlineStr">
@@ -19193,7 +19193,7 @@
       </c>
       <c r="D552" t="inlineStr">
         <is>
-          <t>Wireless Customer Telco Ready</t>
+          <t>Wireless Customer NTP</t>
         </is>
       </c>
       <c r="E552" t="n">
@@ -19217,21 +19217,21 @@
       </c>
       <c r="B553" t="inlineStr">
         <is>
-          <t>Wireless_Distance_from_fiber_feet__c</t>
+          <t>Wireless_Customer_Telco_Ready__c</t>
         </is>
       </c>
       <c r="C553" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>date</t>
         </is>
       </c>
       <c r="D553" t="inlineStr">
         <is>
-          <t>Wireless Distance from fiber (feet)</t>
+          <t>Wireless Customer Telco Ready</t>
         </is>
       </c>
       <c r="E553" t="n">
-        <v>140</v>
+        <v>0</v>
       </c>
       <c r="F553" t="b">
         <v>1</v>
@@ -19251,7 +19251,7 @@
       </c>
       <c r="B554" t="inlineStr">
         <is>
-          <t>Wireless_Entity__c</t>
+          <t>Wireless_Distance_from_fiber_feet__c</t>
         </is>
       </c>
       <c r="C554" t="inlineStr">
@@ -19261,11 +19261,11 @@
       </c>
       <c r="D554" t="inlineStr">
         <is>
-          <t>Wireless Tower Entity</t>
+          <t>Wireless Distance from fiber (feet)</t>
         </is>
       </c>
       <c r="E554" t="n">
-        <v>50</v>
+        <v>140</v>
       </c>
       <c r="F554" t="b">
         <v>1</v>
@@ -19285,21 +19285,21 @@
       </c>
       <c r="B555" t="inlineStr">
         <is>
-          <t>Wireless_Joint_Virtual_Walkout_Complete__c</t>
+          <t>Wireless_Entity__c</t>
         </is>
       </c>
       <c r="C555" t="inlineStr">
         <is>
-          <t>date</t>
+          <t>string</t>
         </is>
       </c>
       <c r="D555" t="inlineStr">
         <is>
-          <t>Wireless Joint/Virtual Walkout Complete</t>
+          <t>Wireless Tower Entity</t>
         </is>
       </c>
       <c r="E555" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F555" t="b">
         <v>1</v>
@@ -19319,7 +19319,7 @@
       </c>
       <c r="B556" t="inlineStr">
         <is>
-          <t>Wireless_List_received__c</t>
+          <t>Wireless_Joint_Virtual_Walkout_Complete__c</t>
         </is>
       </c>
       <c r="C556" t="inlineStr">
@@ -19329,7 +19329,7 @@
       </c>
       <c r="D556" t="inlineStr">
         <is>
-          <t>Wireless List received</t>
+          <t>Wireless Joint/Virtual Walkout Complete</t>
         </is>
       </c>
       <c r="E556" t="n">
@@ -19353,21 +19353,21 @@
       </c>
       <c r="B557" t="inlineStr">
         <is>
-          <t>Wireless_On_Net_Off_Net_Status__c</t>
+          <t>Wireless_List_received__c</t>
         </is>
       </c>
       <c r="C557" t="inlineStr">
         <is>
-          <t>picklist</t>
+          <t>date</t>
         </is>
       </c>
       <c r="D557" t="inlineStr">
         <is>
-          <t>Wireless On Net/Off Net Status</t>
+          <t>Wireless List received</t>
         </is>
       </c>
       <c r="E557" t="n">
-        <v>255</v>
+        <v>0</v>
       </c>
       <c r="F557" t="b">
         <v>1</v>
@@ -19387,21 +19387,21 @@
       </c>
       <c r="B558" t="inlineStr">
         <is>
-          <t>Wireless_Polygon__c</t>
+          <t>Wireless_On_Net_Off_Net_Status__c</t>
         </is>
       </c>
       <c r="C558" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>picklist</t>
         </is>
       </c>
       <c r="D558" t="inlineStr">
         <is>
-          <t>Wireless Polygon (Deprecated)</t>
+          <t>Wireless On Net/Off Net Status</t>
         </is>
       </c>
       <c r="E558" t="n">
-        <v>50</v>
+        <v>255</v>
       </c>
       <c r="F558" t="b">
         <v>1</v>
@@ -19421,21 +19421,21 @@
       </c>
       <c r="B559" t="inlineStr">
         <is>
-          <t>Wireless_Site_Design_Submitted__c</t>
+          <t>Wireless_Polygon__c</t>
         </is>
       </c>
       <c r="C559" t="inlineStr">
         <is>
-          <t>date</t>
+          <t>string</t>
         </is>
       </c>
       <c r="D559" t="inlineStr">
         <is>
-          <t>Wireless Site Design Submitted</t>
+          <t>Wireless Polygon (Deprecated)</t>
         </is>
       </c>
       <c r="E559" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F559" t="b">
         <v>1</v>
@@ -19455,21 +19455,21 @@
       </c>
       <c r="B560" t="inlineStr">
         <is>
-          <t>Wireless_Site__c</t>
+          <t>Wireless_Site_Design_Submitted__c</t>
         </is>
       </c>
       <c r="C560" t="inlineStr">
         <is>
-          <t>picklist</t>
+          <t>date</t>
         </is>
       </c>
       <c r="D560" t="inlineStr">
         <is>
-          <t>Site Selection</t>
+          <t>Wireless Site Design Submitted</t>
         </is>
       </c>
       <c r="E560" t="n">
-        <v>255</v>
+        <v>0</v>
       </c>
       <c r="F560" t="b">
         <v>1</v>
@@ -19489,21 +19489,21 @@
       </c>
       <c r="B561" t="inlineStr">
         <is>
-          <t>LOA_CFA_Complete_Date__c</t>
+          <t>Wireless_Site__c</t>
         </is>
       </c>
       <c r="C561" t="inlineStr">
         <is>
-          <t>date</t>
+          <t>picklist</t>
         </is>
       </c>
       <c r="D561" t="inlineStr">
         <is>
-          <t>Address A: LOA/CFA Complete Date</t>
+          <t>Site Selection</t>
         </is>
       </c>
       <c r="E561" t="n">
-        <v>0</v>
+        <v>255</v>
       </c>
       <c r="F561" t="b">
         <v>1</v>
@@ -19523,7 +19523,7 @@
       </c>
       <c r="B562" t="inlineStr">
         <is>
-          <t>Wireless_Transport_Approval__c</t>
+          <t>LOA_CFA_Complete_Date__c</t>
         </is>
       </c>
       <c r="C562" t="inlineStr">
@@ -19533,7 +19533,7 @@
       </c>
       <c r="D562" t="inlineStr">
         <is>
-          <t>Wireless Transport Approval</t>
+          <t>Address A: LOA/CFA Complete Date</t>
         </is>
       </c>
       <c r="E562" t="n">
@@ -19557,17 +19557,17 @@
       </c>
       <c r="B563" t="inlineStr">
         <is>
-          <t>Customer_Comments_Last_Modified_Date__c</t>
+          <t>Wireless_Transport_Approval__c</t>
         </is>
       </c>
       <c r="C563" t="inlineStr">
         <is>
-          <t>datetime</t>
+          <t>date</t>
         </is>
       </c>
       <c r="D563" t="inlineStr">
         <is>
-          <t>Customer Comments Last Created Date</t>
+          <t>Wireless Transport Approval</t>
         </is>
       </c>
       <c r="E563" t="n">
@@ -19577,7 +19577,7 @@
         <v>1</v>
       </c>
       <c r="G563" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H563" t="b">
         <v>1</v>
@@ -19591,21 +19591,21 @@
       </c>
       <c r="B564" t="inlineStr">
         <is>
-          <t>Opportunity_Service_Category__c</t>
+          <t>Customer_Comments_Last_Modified_Date__c</t>
         </is>
       </c>
       <c r="C564" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>datetime</t>
         </is>
       </c>
       <c r="D564" t="inlineStr">
         <is>
-          <t>Opportunity Service Category</t>
+          <t>Customer Comments Last Created Date</t>
         </is>
       </c>
       <c r="E564" t="n">
-        <v>1300</v>
+        <v>0</v>
       </c>
       <c r="F564" t="b">
         <v>1</v>
@@ -19625,7 +19625,7 @@
       </c>
       <c r="B565" t="inlineStr">
         <is>
-          <t>Opportunity_Stage__c</t>
+          <t>Opportunity_Service_Category__c</t>
         </is>
       </c>
       <c r="C565" t="inlineStr">
@@ -19635,7 +19635,7 @@
       </c>
       <c r="D565" t="inlineStr">
         <is>
-          <t>Opportunity: Stage</t>
+          <t>Opportunity Service Category</t>
         </is>
       </c>
       <c r="E565" t="n">
@@ -19659,27 +19659,27 @@
       </c>
       <c r="B566" t="inlineStr">
         <is>
-          <t>Hold_Reason__c</t>
+          <t>Opportunity_Stage__c</t>
         </is>
       </c>
       <c r="C566" t="inlineStr">
         <is>
-          <t>picklist</t>
+          <t>string</t>
         </is>
       </c>
       <c r="D566" t="inlineStr">
         <is>
-          <t>Hold Reason</t>
+          <t>Opportunity: Stage</t>
         </is>
       </c>
       <c r="E566" t="n">
-        <v>255</v>
+        <v>1300</v>
       </c>
       <c r="F566" t="b">
         <v>1</v>
       </c>
       <c r="G566" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H566" t="b">
         <v>1</v>
@@ -19693,27 +19693,27 @@
       </c>
       <c r="B567" t="inlineStr">
         <is>
-          <t>Address_A_Type_of_Building__c</t>
+          <t>Hold_Reason__c</t>
         </is>
       </c>
       <c r="C567" t="inlineStr">
         <is>
-          <t>string</t>
+          <t>picklist</t>
         </is>
       </c>
       <c r="D567" t="inlineStr">
         <is>
-          <t>Address A: Type of Building</t>
+          <t>Hold Reason</t>
         </is>
       </c>
       <c r="E567" t="n">
-        <v>1300</v>
+        <v>255</v>
       </c>
       <c r="F567" t="b">
         <v>1</v>
       </c>
       <c r="G567" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H567" t="b">
         <v>1</v>
@@ -19727,27 +19727,27 @@
       </c>
       <c r="B568" t="inlineStr">
         <is>
-          <t>Confirmed_FOC_Date__c</t>
+          <t>Address_A_Type_of_Building__c</t>
         </is>
       </c>
       <c r="C568" t="inlineStr">
         <is>
-          <t>date</t>
+          <t>string</t>
         </is>
       </c>
       <c r="D568" t="inlineStr">
         <is>
-          <t>Confirmed FOC Date (Off-Net Only)</t>
+          <t>Address A: Type of Building</t>
         </is>
       </c>
       <c r="E568" t="n">
-        <v>0</v>
+        <v>1300</v>
       </c>
       <c r="F568" t="b">
         <v>1</v>
       </c>
       <c r="G568" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H568" t="b">
         <v>1</v>
@@ -19761,7 +19761,7 @@
       </c>
       <c r="B569" t="inlineStr">
         <is>
-          <t>Target_FOC_Date__c</t>
+          <t>Confirmed_FOC_Date__c</t>
         </is>
       </c>
       <c r="C569" t="inlineStr">
@@ -19771,7 +19771,7 @@
       </c>
       <c r="D569" t="inlineStr">
         <is>
-          <t>Target FOC Date</t>
+          <t>Confirmed FOC Date (Off-Net Only)</t>
         </is>
       </c>
       <c r="E569" t="n">
@@ -19781,7 +19781,7 @@
         <v>1</v>
       </c>
       <c r="G569" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H569" t="b">
         <v>1</v>
@@ -19795,7 +19795,7 @@
       </c>
       <c r="B570" t="inlineStr">
         <is>
-          <t>ISP_Completion__c</t>
+          <t>Target_FOC_Date__c</t>
         </is>
       </c>
       <c r="C570" t="inlineStr">
@@ -19805,7 +19805,7 @@
       </c>
       <c r="D570" t="inlineStr">
         <is>
-          <t>ISP Complete Date (DL)</t>
+          <t>Target FOC Date</t>
         </is>
       </c>
       <c r="E570" t="n">
@@ -19815,7 +19815,7 @@
         <v>1</v>
       </c>
       <c r="G570" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H570" t="b">
         <v>1</v>
@@ -19829,7 +19829,7 @@
       </c>
       <c r="B571" t="inlineStr">
         <is>
-          <t>Projected_Telco_Ready__c</t>
+          <t>ISP_Completion__c</t>
         </is>
       </c>
       <c r="C571" t="inlineStr">
@@ -19839,7 +19839,7 @@
       </c>
       <c r="D571" t="inlineStr">
         <is>
-          <t>Projected Telco Ready</t>
+          <t>ISP Complete Date (DL)</t>
         </is>
       </c>
       <c r="E571" t="n">
@@ -19863,7 +19863,7 @@
       </c>
       <c r="B572" t="inlineStr">
         <is>
-          <t>Order_Confirmation_FOC__c</t>
+          <t>Projected_Telco_Ready__c</t>
         </is>
       </c>
       <c r="C572" t="inlineStr">
@@ -19873,7 +19873,7 @@
       </c>
       <c r="D572" t="inlineStr">
         <is>
-          <t>Order Confirmation FOC</t>
+          <t>Projected Telco Ready</t>
         </is>
       </c>
       <c r="E572" t="n">
@@ -19897,24 +19897,24 @@
       </c>
       <c r="B573" t="inlineStr">
         <is>
-          <t>Force_Resource_Sync__c</t>
+          <t>Order_Confirmation_FOC__c</t>
         </is>
       </c>
       <c r="C573" t="inlineStr">
         <is>
-          <t>boolean</t>
+          <t>date</t>
         </is>
       </c>
       <c r="D573" t="inlineStr">
         <is>
-          <t>Force Resource Sync to the Project</t>
+          <t>Order Confirmation FOC</t>
         </is>
       </c>
       <c r="E573" t="n">
         <v>0</v>
       </c>
       <c r="F573" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G573" t="b">
         <v>0</v>
@@ -19931,27 +19931,27 @@
       </c>
       <c r="B574" t="inlineStr">
         <is>
-          <t>Permits_Approved__c</t>
+          <t>Force_Resource_Sync__c</t>
         </is>
       </c>
       <c r="C574" t="inlineStr">
         <is>
-          <t>percent</t>
+          <t>boolean</t>
         </is>
       </c>
       <c r="D574" t="inlineStr">
         <is>
-          <t>% Permits Approved</t>
+          <t>Force Resource Sync to the Project</t>
         </is>
       </c>
       <c r="E574" t="n">
         <v>0</v>
       </c>
       <c r="F574" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G574" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H574" t="b">
         <v>1</v>
@@ -19965,17 +19965,17 @@
       </c>
       <c r="B575" t="inlineStr">
         <is>
-          <t>Order_Completion_Notice_Sent__c</t>
+          <t>Permits_Approved__c</t>
         </is>
       </c>
       <c r="C575" t="inlineStr">
         <is>
-          <t>date</t>
+          <t>percent</t>
         </is>
       </c>
       <c r="D575" t="inlineStr">
         <is>
-          <t>Order Completion Notice Sent</t>
+          <t>% Permits Approved</t>
         </is>
       </c>
       <c r="E575" t="n">
@@ -19985,7 +19985,7 @@
         <v>1</v>
       </c>
       <c r="G575" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H575" t="b">
         <v>1</v>
@@ -19999,21 +19999,21 @@
       </c>
       <c r="B576" t="inlineStr">
         <is>
-          <t>Pole_Build_Type__c</t>
+          <t>Order_Completion_Notice_Sent__c</t>
         </is>
       </c>
       <c r="C576" t="inlineStr">
         <is>
-          <t>picklist</t>
+          <t>date</t>
         </is>
       </c>
       <c r="D576" t="inlineStr">
         <is>
-          <t>Pole Build Type</t>
+          <t>Order Completion Notice Sent</t>
         </is>
       </c>
       <c r="E576" t="n">
-        <v>255</v>
+        <v>0</v>
       </c>
       <c r="F576" t="b">
         <v>1</v>
@@ -20033,7 +20033,7 @@
       </c>
       <c r="B577" t="inlineStr">
         <is>
-          <t>Pole_Type__c</t>
+          <t>Pole_Build_Type__c</t>
         </is>
       </c>
       <c r="C577" t="inlineStr">
@@ -20043,7 +20043,7 @@
       </c>
       <c r="D577" t="inlineStr">
         <is>
-          <t>Pole Type</t>
+          <t>Pole Build Type</t>
         </is>
       </c>
       <c r="E577" t="n">
@@ -20067,21 +20067,21 @@
       </c>
       <c r="B578" t="inlineStr">
         <is>
-          <t>Pole_Set_Date__c</t>
+          <t>Pole_Type__c</t>
         </is>
       </c>
       <c r="C578" t="inlineStr">
         <is>
-          <t>date</t>
+          <t>picklist</t>
         </is>
       </c>
       <c r="D578" t="inlineStr">
         <is>
-          <t>Pole Set Date</t>
+          <t>Pole Type</t>
         </is>
       </c>
       <c r="E578" t="n">
-        <v>0</v>
+        <v>255</v>
       </c>
       <c r="F578" t="b">
         <v>1</v>
@@ -20101,7 +20101,7 @@
       </c>
       <c r="B579" t="inlineStr">
         <is>
-          <t>Pole_Request_Approved_Date__c</t>
+          <t>Pole_Set_Date__c</t>
         </is>
       </c>
       <c r="C579" t="inlineStr">
@@ -20111,7 +20111,7 @@
       </c>
       <c r="D579" t="inlineStr">
         <is>
-          <t>Pole Request Approved Date</t>
+          <t>Pole Set Date</t>
         </is>
       </c>
       <c r="E579" t="n">
@@ -20135,29 +20135,63 @@
       </c>
       <c r="B580" t="inlineStr">
         <is>
+          <t>Pole_Request_Approved_Date__c</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>date</t>
+        </is>
+      </c>
+      <c r="D580" t="inlineStr">
+        <is>
+          <t>Pole Request Approved Date</t>
+        </is>
+      </c>
+      <c r="E580" t="n">
+        <v>0</v>
+      </c>
+      <c r="F580" t="b">
+        <v>1</v>
+      </c>
+      <c r="G580" t="b">
+        <v>0</v>
+      </c>
+      <c r="H580" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>Order</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
           <t>Pole_Request_Submitted_Date__c</t>
         </is>
       </c>
-      <c r="C580" t="inlineStr">
+      <c r="C581" t="inlineStr">
         <is>
           <t>date</t>
         </is>
       </c>
-      <c r="D580" t="inlineStr">
+      <c r="D581" t="inlineStr">
         <is>
           <t>Pole Request Submitted Date</t>
         </is>
       </c>
-      <c r="E580" t="n">
-        <v>0</v>
-      </c>
-      <c r="F580" t="b">
-        <v>1</v>
-      </c>
-      <c r="G580" t="b">
-        <v>0</v>
-      </c>
-      <c r="H580" t="b">
+      <c r="E581" t="n">
+        <v>0</v>
+      </c>
+      <c r="F581" t="b">
+        <v>1</v>
+      </c>
+      <c r="G581" t="b">
+        <v>0</v>
+      </c>
+      <c r="H581" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>